<commit_message>
Update the features for the latests release
</commit_message>
<xml_diff>
--- a/data/legal_panel_for_government/rm6360/Supplier details.xlsx
+++ b/data/legal_panel_for_government/rm6360/Supplier details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothy.south/Documents/DFP/Test Data/LPG/RM6360/Supplier spreadsheet templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothy.south/Code/crown-marketplace-runner/code/testing/crown-marketplace-feature-tests/data/legal_panel_for_government/rm6360/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA79671-DD1B-AE48-91A5-9BADA9E02F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771DFCF1-B613-7C46-82C0-9A093F897D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1846,7 +1846,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>